<commit_message>
restored repo from github created SmallData_backup from old repo
</commit_message>
<xml_diff>
--- a/backend/model_data/TrainingData_clean_de.xlsx
+++ b/backend/model_data/TrainingData_clean_de.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showSheetTabs="0" xWindow="980" yWindow="460" windowWidth="23620" windowHeight="15460" tabRatio="500"/>
+    <workbookView showSheetTabs="0" xWindow="0" yWindow="460" windowWidth="23620" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12055" uniqueCount="1512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12320" uniqueCount="1577">
   <si>
     <t>User</t>
   </si>
@@ -4657,6 +4657,201 @@
   </si>
   <si>
     <t>FranzBerlin</t>
+  </si>
+  <si>
+    <t>Und warum soll das nicht legitim sein?</t>
+  </si>
+  <si>
+    <t>Im Zweifel hat er oder seine Familie hart für das Geld gearbeitet und dabei schon deutlich höhere Einkommensteuersätze gezahlt als andere.</t>
+  </si>
+  <si>
+    <t>Im Grunde sind das doch alle Neiddebatten von Leuten, die sich darüber ärgern, dass der Nachbar das größere Haus, die hübschere Frau oder das neuere Auto hat</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/wirtschaft/2019-08/vermoegensverteilung-reichtum-finanzen-gerechtigkeit-vermoegenssteuer-mietendeckel</t>
+  </si>
+  <si>
+    <t>Rotrud75</t>
+  </si>
+  <si>
+    <t>circular_reasoning</t>
+  </si>
+  <si>
+    <t>Geldhahn zudrehen!</t>
+  </si>
+  <si>
+    <t>Dort wird Soya angebaut, um es an unsere Tiere in der Tierhaltung zu verfüttern</t>
+  </si>
+  <si>
+    <t>Eine von vielen katastrophalen Auswirkungen von Tierprodukten auf unsere Umwelt</t>
+  </si>
+  <si>
+    <t>Dabei brauchen wir diese nicht, im Gegenteil sogar, Tierprodukte werden mit einer Reihe von den sogenannten Volkskrankheiten in Verbindung gebracht</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/2019-08/brasilien-indigene-voelker-waldbraende-survival-international-ngo</t>
+  </si>
+  <si>
+    <t>yet this</t>
+  </si>
+  <si>
+    <t>Ich bin positiv überrascht vom Lompschers Vorschlag</t>
+  </si>
+  <si>
+    <t>W.Buerger</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/politik/berlins-bausenatorin-legt-gesetzesentwurf-vor-welche-folgen-lompschers-mietendeckel-haben-koennte/24940222.html?utm_source=pocket-newtab</t>
+  </si>
+  <si>
+    <t>Eigentum verpflichtet, steht im Grundgesetz</t>
+  </si>
+  <si>
+    <t>Wenn es für das gesparte Geld null Prozent gibt, der Preis für Gold oder die Aktien rauf und runtergeht, warum soll das bei Immobilien nicht genauso gehen</t>
+  </si>
+  <si>
+    <t>Wenn es wegen Ungerechtigkeit Revolutionen gibt, ist auch alles futsch</t>
+  </si>
+  <si>
+    <t>Inflationen sind auch ein Beispiel</t>
+  </si>
+  <si>
+    <t>Das Leben ist so, dass es keine Sicherheit gibt</t>
+  </si>
+  <si>
+    <t>Und wer seine Immobilie für zu viel Geld gekauft und jetzt das Nachsehen hat, der hat sich eben vertan</t>
+  </si>
+  <si>
+    <t>vor einer Immobilienblase wurde schon länger gewarnt</t>
+  </si>
+  <si>
+    <t>Wenn in Zukunft die Mieter mehr Geld in der Tasche haben, können sie mehr Bioprodukte kaufen</t>
+  </si>
+  <si>
+    <t>im Gegensatz dazu, kann der Immobienbesitzer bei weniger Einnahmen keinen zweiten Porsche oder einen weiteren Brilliantring kaufen</t>
+  </si>
+  <si>
+    <t>bleibt doch gleich für die Wirtschaft</t>
+  </si>
+  <si>
+    <t>Das sind keine Enteignungen, das ist nur die Gerechtigkeit, das ist Volksherrschaft (Demokratie)</t>
+  </si>
+  <si>
+    <t>Wir wissen ja, was im Sozialismus passiert ist und nach der Wende gab es neuen Schwung</t>
+  </si>
+  <si>
+    <t>Und wir wissen, was im Kapitalismus jetzt passiert</t>
+  </si>
+  <si>
+    <t>Ich schlage einen permanten Wechsel vor:</t>
+  </si>
+  <si>
+    <t>30 Jahre Kapitalismus, dann 30 Jahre Sozialismus, dann wieder 30 Jahre Kapitalismus usw.</t>
+  </si>
+  <si>
+    <t>Dann geht die eine Phase immer genau dann zuende, wenn es zu großen Verwerfungen gekommen ist</t>
+  </si>
+  <si>
+    <t>Die Menschen spüren doch jetzt, dass der Kapitalismus gerade die Welt kaputt macht.</t>
+  </si>
+  <si>
+    <t>Er bringt es nicht mehr</t>
+  </si>
+  <si>
+    <t>Wir brauchen neuen Schwung, dieses Mal wieder in die andere Richtung</t>
+  </si>
+  <si>
+    <t>gut so Frau Lompscher</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/digital/mobil/2019-08/fairphone-3-smartphone-android-nachhaltigkeit-umwelt/seite-3</t>
+  </si>
+  <si>
+    <t>Ein iphone hält auch mindestens 3, mit Akkutausch 5-6 Jahre</t>
+  </si>
+  <si>
+    <t>Fragt sich, was nachhaltiger ist</t>
+  </si>
+  <si>
+    <t>Miene Baya</t>
+  </si>
+  <si>
+    <t>Und was genau passiert mit diesem Geld aus dem Ablasshandel?</t>
+  </si>
+  <si>
+    <t>https://www.welt.de/reise/nah/article199673298/Fluege-Schweden-reden-nicht-nur-von-Flugscham-sie-tun-etwas.html?utm_source=pocket-newtab</t>
+  </si>
+  <si>
+    <t>Wilhelm D.</t>
+  </si>
+  <si>
+    <t>Wer bekommt das und was wird damit gemacht?</t>
+  </si>
+  <si>
+    <t>BTW: Dass der Klimawandel “ menschengemacht” ist, konnte bislang nicht bewiesen werden</t>
+  </si>
+  <si>
+    <t>https://www.tagesspiegel.de/berlin/gelaendewagen-in-der-stadt-mein-mann-fand-einen-kombi-zu-spiessig/7339948.html</t>
+  </si>
+  <si>
+    <t>Die Frau ist symphatisch!</t>
+  </si>
+  <si>
+    <t>Halloballo241</t>
+  </si>
+  <si>
+    <t>ich musste lachen und nicken, alles was die frau sagt stimmt</t>
+  </si>
+  <si>
+    <t>i agree</t>
+  </si>
+  <si>
+    <t>herrlich wie sie sich über die Ökos und linksgrünen neider lustig macht</t>
+  </si>
+  <si>
+    <t>aber genau so denkt der durchschnittsdeutsche</t>
+  </si>
+  <si>
+    <t>diese belehrungen mit erhobenem zeigefinger gibts eben gerade in szenebezirken berlins</t>
+  </si>
+  <si>
+    <t>aber zum glück nur da</t>
+  </si>
+  <si>
+    <t>dennoch denken diese waldorf-mütter und väter sie würden robin hood für alle anderen spielen</t>
+  </si>
+  <si>
+    <t>Der porsche cayenne ist ein bestes beispiel für neid</t>
+  </si>
+  <si>
+    <t>Das fahrzeug ist nicht deshalb teilweise verpönt weil es groß ist, sondern weil es teuer ist</t>
+  </si>
+  <si>
+    <t>die länge ist dann nur ein scheinheiliges argument um den besitzer zu beschimpfen</t>
+  </si>
+  <si>
+    <t>Fakt: Länge Porsche Cayenne 4,70</t>
+  </si>
+  <si>
+    <t>Länge VW Sharan (klassisches Familienauto)4,80</t>
+  </si>
+  <si>
+    <t>Aktueller Passat: 4,80</t>
+  </si>
+  <si>
+    <t>Wenn ich ein solches fahrzeug hätte würde ich mit freude durch friedrichshain und den prenzelberg fahren und möglichst viele gutmenschen provozieren, die nichtmal den führerschein bestanden haben</t>
+  </si>
+  <si>
+    <t>und dann aufklären dass sie lieber gegen was anderes protestieren sollten (zb. braunkohle)</t>
+  </si>
+  <si>
+    <t>(nicht ganz ernstgemeint)</t>
+  </si>
+  <si>
+    <t>außerdem: kann mir bitte mal jemand erklären, warum gerade die fahrradfahrer sich ständig um das angeblich knapper werdende öl sorgen?</t>
+  </si>
+  <si>
+    <t>die brauchen doch eh keines!</t>
   </si>
 </sst>
 </file>
@@ -5078,12 +5273,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P1040"/>
+  <dimension ref="B1:P1091"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="E1" colorId="8" zoomScale="142" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1022" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="M1" colorId="8" zoomScale="166" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1073" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E1040" sqref="E1040"/>
+      <selection pane="bottomLeft" activeCell="M1075" sqref="M1075"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43352,6 +43547,903 @@
         <v>1497</v>
       </c>
     </row>
+    <row r="1041" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1041" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1041" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D1041" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E1041" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1041" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G1041" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1041" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1041" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="J1041" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="K1041" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="L1041" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M1041" t="s">
+        <v>1512</v>
+      </c>
+      <c r="N1041" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="O1041" s="1" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="1042" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1042" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1042" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D1042" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E1042" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1042" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G1042" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="H1042" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1042" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="J1042" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1042" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1042" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="M1042" t="s">
+        <v>1513</v>
+      </c>
+      <c r="N1042" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="O1042" s="1" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="1043" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1043" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1043" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D1043" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E1043" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1043" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G1043" s="5" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H1043" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1043" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="J1043" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="K1043" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1043" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="M1043" t="s">
+        <v>1514</v>
+      </c>
+      <c r="N1043" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1043" s="1" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="1044" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1044" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1044" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1044" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1044" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="M1044" t="s">
+        <v>1518</v>
+      </c>
+      <c r="N1044" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="O1044" s="1" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="1045" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1045" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1045" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1045" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1045" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1045" t="s">
+        <v>1519</v>
+      </c>
+      <c r="N1045" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="O1045" s="1" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="1046" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1046" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1046" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1046" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1046" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="M1046" t="s">
+        <v>1520</v>
+      </c>
+      <c r="N1046" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="O1046" s="1" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="1047" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1047" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1047" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1047" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1047" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="M1047" t="s">
+        <v>1521</v>
+      </c>
+      <c r="N1047" s="1" t="s">
+        <v>1523</v>
+      </c>
+      <c r="O1047" s="1" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="1048" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1048" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1048" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1048" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="J1048" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1048" t="s">
+        <v>1524</v>
+      </c>
+      <c r="O1048" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1049" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1049" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1049" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1049" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="J1049" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1049" t="s">
+        <v>1527</v>
+      </c>
+      <c r="O1049" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1050" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1050" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1050" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1050" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1050" t="s">
+        <v>1528</v>
+      </c>
+      <c r="O1050" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1051" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1051" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1051" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1051" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1051" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O1051" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1052" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1052" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1052" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1052" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1052" t="s">
+        <v>1530</v>
+      </c>
+      <c r="O1052" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1053" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1053" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1053" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1053" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1053" t="s">
+        <v>1531</v>
+      </c>
+      <c r="O1053" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1054" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1054" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1054" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1054" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1054" t="s">
+        <v>1532</v>
+      </c>
+      <c r="O1054" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1055" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1055" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1055" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1055" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1055" t="s">
+        <v>1533</v>
+      </c>
+      <c r="O1055" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1056" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1056" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1056" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1056" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1056" t="s">
+        <v>1534</v>
+      </c>
+      <c r="O1056" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1057" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1057" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1057" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1057" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1057" t="s">
+        <v>1535</v>
+      </c>
+      <c r="O1057" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1058" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1058" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1058" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1058" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1058" t="s">
+        <v>1536</v>
+      </c>
+      <c r="O1058" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1059" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1059" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1059" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1059" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1059" t="s">
+        <v>1537</v>
+      </c>
+      <c r="O1059" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1060" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1060" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1060" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1060" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1060" t="s">
+        <v>1538</v>
+      </c>
+      <c r="O1060" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1061" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1061" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1061" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1061" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1061" t="s">
+        <v>1539</v>
+      </c>
+      <c r="O1061" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1062" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1062" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1062" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1062" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1062" t="s">
+        <v>1540</v>
+      </c>
+      <c r="O1062" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1063" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1063" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1063" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1063" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1063" t="s">
+        <v>1541</v>
+      </c>
+      <c r="O1063" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1064" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1064" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1064" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1064" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1064" t="s">
+        <v>1542</v>
+      </c>
+      <c r="O1064" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1065" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1065" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1065" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1065" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1065" t="s">
+        <v>1543</v>
+      </c>
+      <c r="O1065" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1066" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1066" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1066" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1066" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1066" t="s">
+        <v>1544</v>
+      </c>
+      <c r="O1066" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1067" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1067" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1067" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1067" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1067" t="s">
+        <v>1545</v>
+      </c>
+      <c r="O1067" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1068" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1068" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1068" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D1068" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="M1068" t="s">
+        <v>1546</v>
+      </c>
+      <c r="O1068" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1069" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1069" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D1069" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="M1069" t="s">
+        <v>1548</v>
+      </c>
+      <c r="O1069" s="1" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="1070" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1070" t="s">
+        <v>1549</v>
+      </c>
+      <c r="O1070" s="1" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="1071" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C1071" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D1071" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1071" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1071" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1071" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1072" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G1072" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1072" t="s">
+        <v>1554</v>
+      </c>
+      <c r="O1072" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1073" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G1073" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1073" t="s">
+        <v>1555</v>
+      </c>
+      <c r="O1073" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1074" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1074" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1074" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D1074" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1074" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1074" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1074" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="H1074" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1074" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1074" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1074" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="L1074" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1074" s="7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="N1074" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="O1074" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1075" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1075" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1075" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D1075" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1075" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1075" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1075" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="H1075" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1075" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1075" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1075" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L1075" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="M1075" t="s">
+        <v>1559</v>
+      </c>
+      <c r="N1075" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="O1075" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1076" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1076" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1076" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D1076" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1076" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1076" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G1076" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="H1076" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1076" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1076" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1076" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1076" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1076" t="s">
+        <v>1561</v>
+      </c>
+      <c r="N1076" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1076" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1077" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B1077" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1077" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D1077" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1077" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1077" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1077" s="5" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H1077" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1077" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1077" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="K1077" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1077" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="M1077" t="s">
+        <v>1562</v>
+      </c>
+      <c r="N1077" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="O1077" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1078" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1078" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="1079" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1079" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="1080" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1080" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="1081" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1081" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="1082" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1082" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="1083" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1083" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1084" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1084" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="1085" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1085" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="1086" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1086" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="1087" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1087" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="1088" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M1088" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="1089" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M1089" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="1090" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M1090" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="1091" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M1091" t="s">
+        <v>1576</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>